<commit_message>
Trying to solve the phase jitter problem
</commit_message>
<xml_diff>
--- a/documents/任意波形发生器对比.xlsx
+++ b/documents/任意波形发生器对比.xlsx
@@ -270,9 +270,6 @@
     <t>3.5 mVpp - 3.6 Vpp</t>
   </si>
   <si>
-    <t>取决于分配BRAM的大小</t>
-  </si>
-  <si>
     <t>现有矩形波、锯齿波、正弦波、DC和任意波形</t>
   </si>
   <si>
@@ -286,13 +283,33 @@
   </si>
   <si>
     <t>自主开发</t>
+  </si>
+  <si>
+    <t>取决于分配BRAM或DDR3存储器的大小</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="4">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,25 +370,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -689,151 +707,153 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="32.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="14" style="10" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="21" style="10" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="10" customWidth="1"/>
+    <col min="9" max="9" width="32.7109375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="10" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="3"/>
+    <col min="14" max="14" width="15.28515625" style="10" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="45">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="1"/>
       <c r="O2" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="45">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="1" t="s">
         <v>58</v>
       </c>
       <c r="O3" s="5" t="s">
@@ -841,46 +861,46 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="60" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="O4" s="4" t="s">
@@ -888,47 +908,47 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="60">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="1"/>
       <c r="O5" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="9" customFormat="1" ht="30">
+    <row r="6" spans="1:15" s="9" customFormat="1" ht="45">
       <c r="A6" s="6" t="s">
         <v>74</v>
       </c>
@@ -951,104 +971,104 @@
         <v>79</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>27</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="O6" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="60">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N7" s="2"/>
+      <c r="N7" s="1"/>
       <c r="O7" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="60">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>24</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="1"/>
       <c r="O8" s="5" t="s">
         <v>48</v>
       </c>

</xml_diff>